<commit_message>
New metadata generated and links updated in constructor args lez go
</commit_message>
<xml_diff>
--- a/02-DApp/backend/pinata/athletes.xlsx
+++ b/02-DApp/backend/pinata/athletes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henryborska/Desktop/Momint/momint/02-DApp/backend/pinata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{648B3054-D784-C14B-9FF9-EC4837E4869C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3ED9E65C-AEAF-0746-BBE7-5CC764232649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -890,7 +890,7 @@
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -901,7 +901,7 @@
     <col min="6" max="6" width="69.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" ht="18">
       <c r="A1" s="8"/>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -914,7 +914,7 @@
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" ht="16">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Adjusted metadata for roster changes
</commit_message>
<xml_diff>
--- a/02-DApp/backend/pinata/athletes.xlsx
+++ b/02-DApp/backend/pinata/athletes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henryborska/Desktop/Momint/momint/02-DApp/backend/pinata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3ED9E65C-AEAF-0746-BBE7-5CC764232649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43848FA9-0760-814E-B84A-93D1DF49CC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -208,12 +208,6 @@
     <t>toucouille plays mid laner for FlyQuest. In 2021, his spring regular-season performances earned him the LFL Spring Split MVP title.</t>
   </si>
   <si>
-    <t>Arrow</t>
-  </si>
-  <si>
-    <t>Noh Dong-hyeon</t>
-  </si>
-  <si>
     <t>Johnsun</t>
   </si>
   <si>
@@ -457,9 +451,6 @@
     <t>PowerOfEvil plays mid laner for Immortals. Famous for his Orianna and his unique build on her (Nashor's Tooth). His ID comes from Warcraft III.</t>
   </si>
   <si>
-    <t>Arrow plays bot laner for Immortals. Known for his incredible mechanics, he is one of the few Korean AD carries to have played Draven in competitive play and also have Draven banned against him.</t>
-  </si>
-  <si>
     <t>Lee Dong-geun</t>
   </si>
   <si>
@@ -550,9 +541,6 @@
     <t>Lawrence Hui</t>
   </si>
   <si>
-    <t>Lost plays bot laner for Golden Guardians. He is the first New Zealand player to compete outside of the OPL. He recorded a pentakill in March 2021 against Cloud9.</t>
-  </si>
-  <si>
     <t>Olleh</t>
   </si>
   <si>
@@ -560,13 +548,25 @@
   </si>
   <si>
     <t>Olleh plays support for Golden Guardians. He reached Rank 1 in Solo Ranked in the Brazilian, Taiwanese and NA servers. Best known for his Morgana throughout his career, and his Tahm Kench after joining Team Liquid.</t>
+  </si>
+  <si>
+    <t>Stixxay</t>
+  </si>
+  <si>
+    <t>Lost now plays bot laner for Immortals after a recent roster change. He is the first New Zealand player to compete outside of the OPL. He recorded a pentakill in March 2021 against Cloud9.</t>
+  </si>
+  <si>
+    <t>Trevor Hayes</t>
+  </si>
+  <si>
+    <t>Stixxay recently replaced Lost on Golden Guardians. He is a talented bot laner from the U.S. His ID Stixxay is based on a band named "StixNStonez" and his first main champion was Katarina.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -608,6 +608,13 @@
       <color rgb="FF222222"/>
       <name val="Rubik"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -635,7 +642,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -652,6 +659,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -890,7 +906,7 @@
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -994,10 +1010,10 @@
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>50</v>
@@ -1009,16 +1025,16 @@
         <v>24</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>17</v>
@@ -1030,16 +1046,16 @@
         <v>24</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>46</v>
@@ -1051,28 +1067,28 @@
         <v>24</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:14" ht="29">
       <c r="A8" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G8" s="1"/>
       <c r="J8" s="8"/>
@@ -1083,22 +1099,22 @@
     </row>
     <row r="9" spans="1:14" ht="43">
       <c r="A9" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G9" s="1"/>
       <c r="J9" s="2"/>
@@ -1108,23 +1124,23 @@
       <c r="N9" s="2"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="A10" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>145</v>
+      <c r="F10" s="14" t="s">
+        <v>177</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1136,22 +1152,22 @@
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="7"/>
@@ -1162,23 +1178,23 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>175</v>
+      <c r="A12" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>178</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>176</v>
+      <c r="F12" s="11" t="s">
+        <v>179</v>
       </c>
       <c r="G12" s="1"/>
       <c r="J12" s="1"/>
@@ -1268,10 +1284,10 @@
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>17</v>
@@ -1283,7 +1299,7 @@
         <v>15</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G16" s="1"/>
       <c r="J16" s="1"/>
@@ -1294,10 +1310,10 @@
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>46</v>
@@ -1309,7 +1325,7 @@
         <v>15</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G17" s="1"/>
       <c r="J17" s="1"/>
@@ -1320,52 +1336,52 @@
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>57</v>
@@ -1377,50 +1393,50 @@
         <v>15</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G22" s="1"/>
     </row>
@@ -1490,10 +1506,10 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>17</v>
@@ -1505,16 +1521,16 @@
         <v>20</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>46</v>
@@ -1526,59 +1542,59 @@
         <v>20</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>57</v>
@@ -1590,49 +1606,49 @@
         <v>20</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G32" s="1"/>
     </row>
@@ -1681,10 +1697,10 @@
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>50</v>
@@ -1696,16 +1712,16 @@
         <v>12</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G35" s="1"/>
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>17</v>
@@ -1717,16 +1733,16 @@
         <v>12</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>46</v>
@@ -1738,49 +1754,49 @@
         <v>12</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G38" s="1"/>
     </row>
     <row r="39" spans="1:8" ht="15.75" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G39" s="1"/>
     </row>
@@ -1789,7 +1805,7 @@
         <v>53</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>57</v>
@@ -1801,50 +1817,50 @@
         <v>12</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="6"/>
     </row>
     <row r="41" spans="1:8" ht="15.75" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G41" s="1"/>
     </row>
     <row r="42" spans="1:8" ht="15.75" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G42" s="1"/>
     </row>
@@ -1915,10 +1931,10 @@
     </row>
     <row r="46" spans="1:8" ht="28">
       <c r="A46" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>17</v>
@@ -1930,16 +1946,16 @@
         <v>10</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G46" s="1"/>
     </row>
     <row r="47" spans="1:8" ht="15.75" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>46</v>
@@ -1951,58 +1967,58 @@
         <v>10</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G47" s="1"/>
     </row>
     <row r="48" spans="1:8" ht="15.75" customHeight="1">
       <c r="A48" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G48" s="1"/>
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1">
       <c r="A49" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G49" s="1"/>
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1">
       <c r="A50" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>57</v>
@@ -2014,49 +2030,49 @@
         <v>10</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G50" s="1"/>
     </row>
     <row r="51" spans="1:7" ht="14">
       <c r="A51" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G51" s="1"/>
     </row>
     <row r="52" spans="1:7" ht="42">
       <c r="A52" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G52" s="1"/>
     </row>

</xml_diff>